<commit_message>
Sector PASSENGER completed - Added soft-mobility - Improved vehicle speed - Long and short travel - Added "choke" constraints
</commit_message>
<xml_diff>
--- a/data/zenodo_ivan/CHE_country_general.xlsx
+++ b/data/zenodo_ivan/CHE_country_general.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/Downloads/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/zenodo_ivan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619A4704-54FD-6042-80FE-F85A1D9056F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F536FC-676F-8C49-BDD5-012DE19E01AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="82">
   <si>
     <t>Name:</t>
   </si>
@@ -264,6 +264,21 @@
   </si>
   <si>
     <t>https://data.worldbank.org/indicator/NY.GDP.MKTP.KD?locations=CH</t>
+  </si>
+  <si>
+    <t>daily_travel_time</t>
+  </si>
+  <si>
+    <t>https://www.are.admin.ch/are/de/home/mobilitaet/grundlagen-und-daten/mzmv.html</t>
+  </si>
+  <si>
+    <t>Federal Office for Spatial Development, Mobility and Transport Microcensus 2021</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>Table G3.2.2.1, includes waiting times</t>
   </si>
 </sst>
 </file>
@@ -699,11 +714,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M217"/>
+  <dimension ref="A1:L250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C178" sqref="C178"/>
+      <pane ySplit="5" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C222" sqref="C222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5858,7 +5873,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>16</v>
       </c>
@@ -5875,7 +5890,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>16</v>
       </c>
@@ -5892,7 +5907,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>16</v>
       </c>
@@ -5909,7 +5924,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>16</v>
       </c>
@@ -5926,7 +5941,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>16</v>
       </c>
@@ -5943,7 +5958,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>16</v>
       </c>
@@ -5960,7 +5975,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>16</v>
       </c>
@@ -5977,7 +5992,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>16</v>
       </c>
@@ -5994,7 +6009,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>16</v>
       </c>
@@ -6011,7 +6026,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>16</v>
       </c>
@@ -6028,7 +6043,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>16</v>
       </c>
@@ -6045,7 +6060,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="188" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>16</v>
       </c>
@@ -6073,11 +6088,11 @@
       <c r="K188" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M188" t="s">
+      <c r="L188" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="189" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>16</v>
       </c>
@@ -6105,11 +6120,11 @@
       <c r="K189" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M189" t="s">
+      <c r="L189" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>16</v>
       </c>
@@ -6137,11 +6152,11 @@
       <c r="K190" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M190" t="s">
+      <c r="L190" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="191" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>16</v>
       </c>
@@ -6169,11 +6184,11 @@
       <c r="K191" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M191" t="s">
+      <c r="L191" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="192" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>16</v>
       </c>
@@ -6201,11 +6216,11 @@
       <c r="K192" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M192" t="s">
+      <c r="L192" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="193" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>16</v>
       </c>
@@ -6233,11 +6248,11 @@
       <c r="K193" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M193" t="s">
+      <c r="L193" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="194" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>16</v>
       </c>
@@ -6265,11 +6280,11 @@
       <c r="K194" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M194" t="s">
+      <c r="L194" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="195" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>16</v>
       </c>
@@ -6297,11 +6312,11 @@
       <c r="K195" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M195" t="s">
+      <c r="L195" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="196" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>16</v>
       </c>
@@ -6329,11 +6344,11 @@
       <c r="K196" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M196" t="s">
+      <c r="L196" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="197" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>16</v>
       </c>
@@ -6361,11 +6376,11 @@
       <c r="K197" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M197" t="s">
+      <c r="L197" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="198" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>16</v>
       </c>
@@ -6393,11 +6408,11 @@
       <c r="K198" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M198" t="s">
+      <c r="L198" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>16</v>
       </c>
@@ -6425,11 +6440,11 @@
       <c r="K199" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M199" t="s">
+      <c r="L199" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="200" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>16</v>
       </c>
@@ -6457,11 +6472,11 @@
       <c r="K200" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M200" t="s">
+      <c r="L200" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="201" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>16</v>
       </c>
@@ -6489,11 +6504,11 @@
       <c r="K201" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M201" t="s">
+      <c r="L201" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="202" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>16</v>
       </c>
@@ -6521,11 +6536,11 @@
       <c r="K202" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M202" t="s">
+      <c r="L202" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="203" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>16</v>
       </c>
@@ -6553,11 +6568,11 @@
       <c r="K203" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M203" t="s">
+      <c r="L203" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="204" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>16</v>
       </c>
@@ -6585,11 +6600,11 @@
       <c r="K204" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M204" t="s">
+      <c r="L204" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="205" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>16</v>
       </c>
@@ -6617,11 +6632,11 @@
       <c r="K205" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M205" t="s">
+      <c r="L205" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="206" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>16</v>
       </c>
@@ -6649,11 +6664,11 @@
       <c r="K206" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M206" t="s">
+      <c r="L206" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="207" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>16</v>
       </c>
@@ -6681,11 +6696,11 @@
       <c r="K207" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M207" t="s">
+      <c r="L207" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>16</v>
       </c>
@@ -6713,11 +6728,11 @@
       <c r="K208" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M208" t="s">
+      <c r="L208" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="209" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>16</v>
       </c>
@@ -6745,11 +6760,11 @@
       <c r="K209" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M209" t="s">
+      <c r="L209" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="210" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>16</v>
       </c>
@@ -6777,11 +6792,11 @@
       <c r="K210" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M210" t="s">
+      <c r="L210" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="211" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>16</v>
       </c>
@@ -6809,11 +6824,11 @@
       <c r="K211" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M211" t="s">
+      <c r="L211" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="212" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>16</v>
       </c>
@@ -6841,11 +6856,11 @@
       <c r="K212" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M212" t="s">
+      <c r="L212" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="213" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>16</v>
       </c>
@@ -6873,11 +6888,11 @@
       <c r="K213" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M213" t="s">
+      <c r="L213" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="214" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>16</v>
       </c>
@@ -6905,11 +6920,11 @@
       <c r="K214" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M214" t="s">
+      <c r="L214" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="215" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>16</v>
       </c>
@@ -6937,11 +6952,11 @@
       <c r="K215" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M215" t="s">
+      <c r="L215" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="216" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>16</v>
       </c>
@@ -6969,11 +6984,11 @@
       <c r="K216" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M216" t="s">
+      <c r="L216" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="217" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>16</v>
       </c>
@@ -7001,9 +7016,705 @@
       <c r="K217" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M217" t="s">
+      <c r="L217" t="s">
         <v>73</v>
       </c>
+    </row>
+    <row r="218" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>16</v>
+      </c>
+      <c r="B218" t="s">
+        <v>22</v>
+      </c>
+      <c r="C218" t="s">
+        <v>77</v>
+      </c>
+      <c r="D218" t="s">
+        <v>18</v>
+      </c>
+      <c r="E218">
+        <v>1990</v>
+      </c>
+      <c r="G218" s="4"/>
+      <c r="K218" s="2"/>
+    </row>
+    <row r="219" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>16</v>
+      </c>
+      <c r="B219" t="s">
+        <v>22</v>
+      </c>
+      <c r="C219" t="s">
+        <v>77</v>
+      </c>
+      <c r="D219" t="s">
+        <v>18</v>
+      </c>
+      <c r="E219">
+        <v>1991</v>
+      </c>
+      <c r="G219" s="4"/>
+      <c r="K219" s="2"/>
+    </row>
+    <row r="220" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>16</v>
+      </c>
+      <c r="B220" t="s">
+        <v>22</v>
+      </c>
+      <c r="C220" t="s">
+        <v>77</v>
+      </c>
+      <c r="D220" t="s">
+        <v>18</v>
+      </c>
+      <c r="E220">
+        <v>1992</v>
+      </c>
+      <c r="G220" s="4"/>
+      <c r="K220" s="2"/>
+    </row>
+    <row r="221" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>16</v>
+      </c>
+      <c r="B221" t="s">
+        <v>22</v>
+      </c>
+      <c r="C221" t="s">
+        <v>77</v>
+      </c>
+      <c r="D221" t="s">
+        <v>18</v>
+      </c>
+      <c r="E221">
+        <v>1993</v>
+      </c>
+      <c r="G221" s="4"/>
+      <c r="K221" s="2"/>
+    </row>
+    <row r="222" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>16</v>
+      </c>
+      <c r="B222" t="s">
+        <v>22</v>
+      </c>
+      <c r="C222" t="s">
+        <v>77</v>
+      </c>
+      <c r="D222" t="s">
+        <v>18</v>
+      </c>
+      <c r="E222">
+        <v>1994</v>
+      </c>
+      <c r="G222" s="4">
+        <f>82.6/60</f>
+        <v>1.3766666666666665</v>
+      </c>
+      <c r="H222" t="s">
+        <v>80</v>
+      </c>
+      <c r="J222" t="s">
+        <v>79</v>
+      </c>
+      <c r="K222" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L222" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>16</v>
+      </c>
+      <c r="B223" t="s">
+        <v>22</v>
+      </c>
+      <c r="C223" t="s">
+        <v>77</v>
+      </c>
+      <c r="D223" t="s">
+        <v>18</v>
+      </c>
+      <c r="E223">
+        <v>1995</v>
+      </c>
+      <c r="G223" s="4"/>
+      <c r="K223" s="2"/>
+    </row>
+    <row r="224" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>16</v>
+      </c>
+      <c r="B224" t="s">
+        <v>22</v>
+      </c>
+      <c r="C224" t="s">
+        <v>77</v>
+      </c>
+      <c r="D224" t="s">
+        <v>18</v>
+      </c>
+      <c r="E224">
+        <v>1996</v>
+      </c>
+      <c r="G224" s="4"/>
+      <c r="K224" s="2"/>
+    </row>
+    <row r="225" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>16</v>
+      </c>
+      <c r="B225" t="s">
+        <v>22</v>
+      </c>
+      <c r="C225" t="s">
+        <v>77</v>
+      </c>
+      <c r="D225" t="s">
+        <v>18</v>
+      </c>
+      <c r="E225">
+        <v>1997</v>
+      </c>
+      <c r="G225" s="4"/>
+      <c r="K225" s="2"/>
+    </row>
+    <row r="226" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>16</v>
+      </c>
+      <c r="B226" t="s">
+        <v>22</v>
+      </c>
+      <c r="C226" t="s">
+        <v>77</v>
+      </c>
+      <c r="D226" t="s">
+        <v>18</v>
+      </c>
+      <c r="E226">
+        <v>1998</v>
+      </c>
+      <c r="G226" s="4"/>
+      <c r="K226" s="2"/>
+    </row>
+    <row r="227" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>16</v>
+      </c>
+      <c r="B227" t="s">
+        <v>22</v>
+      </c>
+      <c r="C227" t="s">
+        <v>77</v>
+      </c>
+      <c r="D227" t="s">
+        <v>18</v>
+      </c>
+      <c r="E227">
+        <v>1999</v>
+      </c>
+      <c r="G227" s="4"/>
+      <c r="K227" s="2"/>
+    </row>
+    <row r="228" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>16</v>
+      </c>
+      <c r="B228" t="s">
+        <v>22</v>
+      </c>
+      <c r="C228" t="s">
+        <v>77</v>
+      </c>
+      <c r="D228" t="s">
+        <v>18</v>
+      </c>
+      <c r="E228">
+        <v>2000</v>
+      </c>
+      <c r="G228" s="4">
+        <f>93.3/60</f>
+        <v>1.5549999999999999</v>
+      </c>
+      <c r="H228" t="s">
+        <v>80</v>
+      </c>
+      <c r="J228" t="s">
+        <v>79</v>
+      </c>
+      <c r="K228" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L228" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>16</v>
+      </c>
+      <c r="B229" t="s">
+        <v>22</v>
+      </c>
+      <c r="C229" t="s">
+        <v>77</v>
+      </c>
+      <c r="D229" t="s">
+        <v>18</v>
+      </c>
+      <c r="E229">
+        <v>2001</v>
+      </c>
+      <c r="G229" s="4"/>
+      <c r="K229" s="2"/>
+    </row>
+    <row r="230" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>16</v>
+      </c>
+      <c r="B230" t="s">
+        <v>22</v>
+      </c>
+      <c r="C230" t="s">
+        <v>77</v>
+      </c>
+      <c r="D230" t="s">
+        <v>18</v>
+      </c>
+      <c r="E230">
+        <v>2002</v>
+      </c>
+      <c r="G230" s="4"/>
+      <c r="K230" s="2"/>
+    </row>
+    <row r="231" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>16</v>
+      </c>
+      <c r="B231" t="s">
+        <v>22</v>
+      </c>
+      <c r="C231" t="s">
+        <v>77</v>
+      </c>
+      <c r="D231" t="s">
+        <v>18</v>
+      </c>
+      <c r="E231">
+        <v>2003</v>
+      </c>
+      <c r="G231" s="4"/>
+      <c r="K231" s="2"/>
+    </row>
+    <row r="232" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>16</v>
+      </c>
+      <c r="B232" t="s">
+        <v>22</v>
+      </c>
+      <c r="C232" t="s">
+        <v>77</v>
+      </c>
+      <c r="D232" t="s">
+        <v>18</v>
+      </c>
+      <c r="E232">
+        <v>2004</v>
+      </c>
+      <c r="G232" s="4"/>
+      <c r="K232" s="2"/>
+    </row>
+    <row r="233" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>16</v>
+      </c>
+      <c r="B233" t="s">
+        <v>22</v>
+      </c>
+      <c r="C233" t="s">
+        <v>77</v>
+      </c>
+      <c r="D233" t="s">
+        <v>18</v>
+      </c>
+      <c r="E233">
+        <v>2005</v>
+      </c>
+      <c r="G233" s="4">
+        <f>97.5/60</f>
+        <v>1.625</v>
+      </c>
+      <c r="H233" t="s">
+        <v>80</v>
+      </c>
+      <c r="J233" t="s">
+        <v>79</v>
+      </c>
+      <c r="K233" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L233" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>16</v>
+      </c>
+      <c r="B234" t="s">
+        <v>22</v>
+      </c>
+      <c r="C234" t="s">
+        <v>77</v>
+      </c>
+      <c r="D234" t="s">
+        <v>18</v>
+      </c>
+      <c r="E234">
+        <v>2006</v>
+      </c>
+      <c r="G234" s="4"/>
+      <c r="K234" s="2"/>
+    </row>
+    <row r="235" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>16</v>
+      </c>
+      <c r="B235" t="s">
+        <v>22</v>
+      </c>
+      <c r="C235" t="s">
+        <v>77</v>
+      </c>
+      <c r="D235" t="s">
+        <v>18</v>
+      </c>
+      <c r="E235">
+        <v>2007</v>
+      </c>
+      <c r="G235" s="4"/>
+      <c r="K235" s="2"/>
+    </row>
+    <row r="236" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>16</v>
+      </c>
+      <c r="B236" t="s">
+        <v>22</v>
+      </c>
+      <c r="C236" t="s">
+        <v>77</v>
+      </c>
+      <c r="D236" t="s">
+        <v>18</v>
+      </c>
+      <c r="E236">
+        <v>2008</v>
+      </c>
+      <c r="G236" s="4"/>
+      <c r="K236" s="2"/>
+    </row>
+    <row r="237" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>16</v>
+      </c>
+      <c r="B237" t="s">
+        <v>22</v>
+      </c>
+      <c r="C237" t="s">
+        <v>77</v>
+      </c>
+      <c r="D237" t="s">
+        <v>18</v>
+      </c>
+      <c r="E237">
+        <v>2009</v>
+      </c>
+      <c r="G237" s="4"/>
+      <c r="K237" s="2"/>
+    </row>
+    <row r="238" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>16</v>
+      </c>
+      <c r="B238" t="s">
+        <v>22</v>
+      </c>
+      <c r="C238" t="s">
+        <v>77</v>
+      </c>
+      <c r="D238" t="s">
+        <v>18</v>
+      </c>
+      <c r="E238">
+        <v>2010</v>
+      </c>
+      <c r="G238" s="4">
+        <f>91.7/60</f>
+        <v>1.5283333333333333</v>
+      </c>
+      <c r="H238" t="s">
+        <v>80</v>
+      </c>
+      <c r="J238" t="s">
+        <v>79</v>
+      </c>
+      <c r="K238" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L238" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>16</v>
+      </c>
+      <c r="B239" t="s">
+        <v>22</v>
+      </c>
+      <c r="C239" t="s">
+        <v>77</v>
+      </c>
+      <c r="D239" t="s">
+        <v>18</v>
+      </c>
+      <c r="E239">
+        <v>2011</v>
+      </c>
+      <c r="G239" s="4"/>
+      <c r="K239" s="2"/>
+    </row>
+    <row r="240" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>16</v>
+      </c>
+      <c r="B240" t="s">
+        <v>22</v>
+      </c>
+      <c r="C240" t="s">
+        <v>77</v>
+      </c>
+      <c r="D240" t="s">
+        <v>18</v>
+      </c>
+      <c r="E240">
+        <v>2012</v>
+      </c>
+      <c r="G240" s="4"/>
+      <c r="K240" s="2"/>
+    </row>
+    <row r="241" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>16</v>
+      </c>
+      <c r="B241" t="s">
+        <v>22</v>
+      </c>
+      <c r="C241" t="s">
+        <v>77</v>
+      </c>
+      <c r="D241" t="s">
+        <v>18</v>
+      </c>
+      <c r="E241">
+        <v>2013</v>
+      </c>
+      <c r="G241" s="4"/>
+      <c r="K241" s="2"/>
+    </row>
+    <row r="242" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>16</v>
+      </c>
+      <c r="B242" t="s">
+        <v>22</v>
+      </c>
+      <c r="C242" t="s">
+        <v>77</v>
+      </c>
+      <c r="D242" t="s">
+        <v>18</v>
+      </c>
+      <c r="E242">
+        <v>2014</v>
+      </c>
+      <c r="G242" s="4"/>
+      <c r="K242" s="2"/>
+    </row>
+    <row r="243" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>16</v>
+      </c>
+      <c r="B243" t="s">
+        <v>22</v>
+      </c>
+      <c r="C243" t="s">
+        <v>77</v>
+      </c>
+      <c r="D243" t="s">
+        <v>18</v>
+      </c>
+      <c r="E243">
+        <v>2015</v>
+      </c>
+      <c r="G243" s="4">
+        <f>90.4/60</f>
+        <v>1.5066666666666668</v>
+      </c>
+      <c r="H243" t="s">
+        <v>80</v>
+      </c>
+      <c r="J243" t="s">
+        <v>79</v>
+      </c>
+      <c r="K243" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L243" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>16</v>
+      </c>
+      <c r="B244" t="s">
+        <v>22</v>
+      </c>
+      <c r="C244" t="s">
+        <v>77</v>
+      </c>
+      <c r="D244" t="s">
+        <v>18</v>
+      </c>
+      <c r="E244">
+        <v>2016</v>
+      </c>
+      <c r="G244" s="4"/>
+      <c r="K244" s="2"/>
+    </row>
+    <row r="245" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>16</v>
+      </c>
+      <c r="B245" t="s">
+        <v>22</v>
+      </c>
+      <c r="C245" t="s">
+        <v>77</v>
+      </c>
+      <c r="D245" t="s">
+        <v>18</v>
+      </c>
+      <c r="E245">
+        <v>2017</v>
+      </c>
+      <c r="G245" s="4"/>
+      <c r="K245" s="2"/>
+    </row>
+    <row r="246" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>16</v>
+      </c>
+      <c r="B246" t="s">
+        <v>22</v>
+      </c>
+      <c r="C246" t="s">
+        <v>77</v>
+      </c>
+      <c r="D246" t="s">
+        <v>18</v>
+      </c>
+      <c r="E246">
+        <v>2018</v>
+      </c>
+      <c r="G246" s="4"/>
+      <c r="K246" s="2"/>
+    </row>
+    <row r="247" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>16</v>
+      </c>
+      <c r="B247" t="s">
+        <v>22</v>
+      </c>
+      <c r="C247" t="s">
+        <v>77</v>
+      </c>
+      <c r="D247" t="s">
+        <v>18</v>
+      </c>
+      <c r="E247">
+        <v>2019</v>
+      </c>
+      <c r="G247" s="4"/>
+      <c r="K247" s="2"/>
+    </row>
+    <row r="248" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>16</v>
+      </c>
+      <c r="B248" t="s">
+        <v>22</v>
+      </c>
+      <c r="C248" t="s">
+        <v>77</v>
+      </c>
+      <c r="D248" t="s">
+        <v>18</v>
+      </c>
+      <c r="E248">
+        <v>2020</v>
+      </c>
+      <c r="G248" s="4"/>
+      <c r="K248" s="2"/>
+    </row>
+    <row r="249" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>16</v>
+      </c>
+      <c r="B249" t="s">
+        <v>22</v>
+      </c>
+      <c r="C249" t="s">
+        <v>77</v>
+      </c>
+      <c r="D249" t="s">
+        <v>18</v>
+      </c>
+      <c r="E249">
+        <v>2021</v>
+      </c>
+      <c r="G249" s="4">
+        <f>80.2/60</f>
+        <v>1.3366666666666667</v>
+      </c>
+      <c r="H249" t="s">
+        <v>80</v>
+      </c>
+      <c r="J249" t="s">
+        <v>79</v>
+      </c>
+      <c r="K249" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L249" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="G250" s="4"/>
+      <c r="K250" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:L570" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>